<commit_message>
02-07-2016: Added the <<definitive>> table with smb and dsmb columns
</commit_message>
<xml_diff>
--- a/output/definitive.xlsx
+++ b/output/definitive.xlsx
@@ -1160,13 +1160,13 @@
         <v>70.7930217292801</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0175177803205931</v>
+        <v>1332.02174797158</v>
       </c>
       <c r="R2" t="n">
-        <v>0.00696457864256505</v>
+        <v>128.396594571143</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.0261780217139557</v>
+        <v>527.365239108085</v>
       </c>
     </row>
     <row r="3">
@@ -1219,13 +1219,13 @@
         <v>13.6187565667187</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.00538253493699337</v>
+        <v>271.176738064172</v>
       </c>
       <c r="R3" t="n">
-        <v>0.00213994508316651</v>
+        <v>27.2287548961168</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.00804349146284801</v>
+        <v>90.2820686613982</v>
       </c>
     </row>
     <row r="4">
@@ -1278,13 +1278,13 @@
         <v>19.8856621901187</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.00425940402330314</v>
+        <v>557.486977037644</v>
       </c>
       <c r="R4" t="n">
-        <v>0.00169341969974814</v>
+        <v>-17.5062372651231</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.00636511983652758</v>
+        <v>60.3196963909475</v>
       </c>
     </row>
     <row r="5">
@@ -1337,13 +1337,13 @@
         <v>3.29495864859462</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.000661522291325094</v>
+        <v>74.9078035724264</v>
       </c>
       <c r="R5" t="n">
-        <v>0.000263002728509353</v>
+        <v>2.21532775454592</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.000988558172876305</v>
+        <v>14.1874301803554</v>
       </c>
     </row>
     <row r="6">
@@ -1396,13 +1396,13 @@
         <v>21.4076598149126</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.00584796029861752</v>
+        <v>379.210613351733</v>
       </c>
       <c r="R6" t="n">
-        <v>0.00232498516666756</v>
+        <v>57.3445139209004</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.00873900853178282</v>
+        <v>157.423922727042</v>
       </c>
     </row>
     <row r="7">
@@ -1455,13 +1455,13 @@
         <v>2.25123431292528</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.000353811451028087</v>
+        <v>54.2147500658909</v>
       </c>
       <c r="R7" t="n">
-        <v>0.00014066551984491</v>
+        <v>5.90009467702878</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.000528724740129966</v>
+        <v>14.3674393437545</v>
       </c>
     </row>
     <row r="8">
@@ -1573,13 +1573,13 @@
         <v>9.55613751829932</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.00313152940068464</v>
+        <v>137.905558514223</v>
       </c>
       <c r="R9" t="n">
-        <v>0.00124500835056906</v>
+        <v>-0.800580838868496</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.00467965936030402</v>
+        <v>-6.12978319284748</v>
       </c>
     </row>
     <row r="10">
@@ -1632,13 +1632,13 @@
         <v>15.9230173291997</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.00246211741479965</v>
+        <v>308.19423633973</v>
       </c>
       <c r="R10" t="n">
-        <v>0.000978868900556032</v>
+        <v>1.65186434146875</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.00367931107522596</v>
+        <v>26.9844711643318</v>
       </c>
     </row>
     <row r="11">
@@ -1691,13 +1691,13 @@
         <v>7.49812638441794</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.000758233443809257</v>
+        <v>142.453816661317</v>
       </c>
       <c r="R11" t="n">
-        <v>0.000301452373085456</v>
+        <v>-3.25833330793488</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.00113308028717271</v>
+        <v>4.07545910988381</v>
       </c>
     </row>
     <row r="12">
@@ -1750,13 +1750,13 @@
         <v>3.98852361724034</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.000638389740331313</v>
+        <v>75.5557164594573</v>
       </c>
       <c r="R12" t="n">
-        <v>0.000253805874361688</v>
+        <v>5.54666441005803</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.000953989613896119</v>
+        <v>16.6315656575833</v>
       </c>
     </row>
     <row r="13">
@@ -1809,13 +1809,13 @@
         <v>1.96565658298567</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.000388935652114534</v>
+        <v>35.9912258445195</v>
       </c>
       <c r="R13" t="n">
-        <v>0.000154629918087549</v>
+        <v>-0.0457932469920995</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.000581213245060323</v>
+        <v>10.9209203065984</v>
       </c>
     </row>
     <row r="14">
@@ -1868,13 +1868,13 @@
         <v>0.276161621538561</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.000223195738685299</v>
+        <v>10.3518975583481</v>
       </c>
       <c r="R14" t="n">
-        <v>0.0000887363722064607</v>
+        <v>-1.43273131319767</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.000333536714517283</v>
+        <v>1.35985423631178</v>
       </c>
     </row>
     <row r="15">
@@ -1927,13 +1927,13 @@
         <v>27.973218291374</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.0100524448062446</v>
+        <v>947.607420535923</v>
       </c>
       <c r="R15" t="n">
-        <v>0.00399657040571707</v>
+        <v>-30.5899985925267</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.0150220583658571</v>
+        <v>54.4490355171217</v>
       </c>
     </row>
     <row r="16">
@@ -1986,13 +1986,13 @@
         <v>29.5866885539514</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0158039966193877</v>
+        <v>1054.39414608325</v>
       </c>
       <c r="R16" t="n">
-        <v>0.00628322625973146</v>
+        <v>-15.3534281790346</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.023616997079434</v>
+        <v>39.3160331292686</v>
       </c>
     </row>
     <row r="17">
@@ -2045,13 +2045,13 @@
         <v>33.5775485292438</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.00284055640794546</v>
+        <v>1012.33120858216</v>
       </c>
       <c r="R17" t="n">
-        <v>0.00112932564113285</v>
+        <v>-2.93678428037042</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.00424483844220251</v>
+        <v>50.8364089339072</v>
       </c>
     </row>
     <row r="18">
@@ -2104,13 +2104,13 @@
         <v>11.9719429209121</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.000750212300806481</v>
+        <v>288.911747433697</v>
       </c>
       <c r="R18" t="n">
-        <v>0.000298263391363815</v>
+        <v>-11.5846466360928</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.00112109374253894</v>
+        <v>29.9184928620856</v>
       </c>
     </row>
     <row r="19">
@@ -2163,13 +2163,13 @@
         <v>3.97531225345787</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.000322652748980093</v>
+        <v>54.2009255134342</v>
       </c>
       <c r="R19" t="n">
-        <v>0.000128277692914668</v>
+        <v>1.59671093444798</v>
       </c>
       <c r="S19" t="n">
-        <v>-0.000482162152640946</v>
+        <v>20.8559894083978</v>
       </c>
     </row>
     <row r="20">
@@ -2222,13 +2222,13 @@
         <v>24.1747992258391</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.00186034138363685</v>
+        <v>569.306070782311</v>
       </c>
       <c r="R20" t="n">
-        <v>0.000739619611117399</v>
+        <v>22.3198947270323</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.00278003584044071</v>
+        <v>156.893005449802</v>
       </c>
     </row>
     <row r="21">
@@ -2281,13 +2281,13 @@
         <v>27.9019163495893</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.00252496453650125</v>
+        <v>529.378878482933</v>
       </c>
       <c r="R21" t="n">
-        <v>0.00100385515529489</v>
+        <v>14.4456597001585</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.00377322784358674</v>
+        <v>168.370424921899</v>
       </c>
     </row>
     <row r="22">
@@ -2340,13 +2340,13 @@
         <v>0.297222919580271</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.0000142935983542642</v>
+        <v>3.50147372735937</v>
       </c>
       <c r="R22" t="n">
-        <v>0.00000568273422783401</v>
+        <v>0.0747662264202085</v>
       </c>
       <c r="S22" t="n">
-        <v>-0.0000213599052642887</v>
+        <v>0.634140848276613</v>
       </c>
     </row>
     <row r="23">
@@ -2399,13 +2399,13 @@
         <v>34.3363663584496</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.00401574952196045</v>
+        <v>1172.06933673294</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0015965494967224</v>
+        <v>21.8761862127158</v>
       </c>
       <c r="S23" t="n">
-        <v>-0.00600101018849451</v>
+        <v>-284.63297006762</v>
       </c>
     </row>
     <row r="24">

</xml_diff>

<commit_message>
Added proper generation of supermask, plotting example.
</commit_message>
<xml_diff>
--- a/output/definitive.xlsx
+++ b/output/definitive.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="232">
   <si>
     <t>Name</t>
   </si>
@@ -275,385 +275,373 @@
     <t>5</t>
   </si>
   <si>
-    <t>Wilma/Robert/Downer + Edward VII</t>
-  </si>
-  <si>
-    <t>14.4</t>
+    <t>Amery</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>50.4</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>-21.4</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>35.5</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Conger + Tracy/Tremenchus + Shackleton + West + Publications</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>69.4</t>
+  </si>
+  <si>
+    <t>25.4</t>
+  </si>
+  <si>
+    <t>-47.1</t>
+  </si>
+  <si>
+    <t>60.8</t>
+  </si>
+  <si>
+    <t>107.6</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
+    <t>11.9</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>23.8</t>
+  </si>
+  <si>
+    <t>17.3</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Holmes + Moscow University + Totten + Vincennes</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>89.1</t>
+  </si>
+  <si>
+    <t>-15.3</t>
+  </si>
+  <si>
+    <t>87.1</t>
+  </si>
+  <si>
+    <t>102.3</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Cook + Ninnis + Mertz + Dibble</t>
+  </si>
+  <si>
+    <t>96.1</t>
+  </si>
+  <si>
+    <t>72.4</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>31.6</t>
+  </si>
+  <si>
+    <t>22.8</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>Aviator + Mariner + Lillie + Rennick</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>Drygalski + Nansen</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>-0.4</t>
+  </si>
+  <si>
+    <t>8.7</t>
   </si>
   <si>
     <t>1.1</t>
   </si>
   <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Ross East</t>
+  </si>
+  <si>
+    <t>56.1</t>
+  </si>
+  <si>
+    <t>45.8</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>-7.8</t>
+  </si>
+  <si>
+    <t>41.3</t>
+  </si>
+  <si>
+    <t>49.1</t>
+  </si>
+  <si>
+    <t>Ross West</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>100.4</t>
+  </si>
+  <si>
+    <t>33.5</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>-1.4</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Getz + Land + Nickerson + Sulzberger + Swinburne + Withrow</t>
+  </si>
+  <si>
+    <t>140.3</t>
+  </si>
+  <si>
+    <t>73.7</t>
+  </si>
+  <si>
+    <t>48.8</t>
+  </si>
+  <si>
+    <t>-59.6</t>
+  </si>
+  <si>
+    <t>115.6</t>
+  </si>
+  <si>
+    <t>175.2</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>15.6</t>
+  </si>
+  <si>
+    <t>19.9</t>
+  </si>
+  <si>
+    <t>Thwaites + Crosson + Dotson</t>
+  </si>
+  <si>
+    <t>169.3</t>
+  </si>
+  <si>
+    <t>71.7</t>
+  </si>
+  <si>
+    <t>-69.5</t>
+  </si>
+  <si>
+    <t>111.7</t>
+  </si>
+  <si>
+    <t>181.2</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Pine Island</t>
+  </si>
+  <si>
+    <t>126.4</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>-33.2</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>101.2</t>
+  </si>
+  <si>
+    <t>Ferrigno + Venable + Abbot + Cosgrove</t>
+  </si>
+  <si>
+    <t>64.8</t>
+  </si>
+  <si>
+    <t>16.8</t>
+  </si>
+  <si>
+    <t>30.2</t>
+  </si>
+  <si>
+    <t>-6.4</t>
+  </si>
+  <si>
+    <t>78.3</t>
+  </si>
+  <si>
+    <t>84.8</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Wilkins + Bach + George VI + Stange</t>
+  </si>
+  <si>
+    <t>102.4</t>
+  </si>
+  <si>
+    <t>28.8</t>
+  </si>
+  <si>
+    <t>-26.8</t>
+  </si>
+  <si>
+    <t>119.4</t>
+  </si>
+  <si>
+    <t>146.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>37.3</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Wordie</t>
+  </si>
+  <si>
+    <t>13.8</t>
+  </si>
+  <si>
+    <t>-0.1</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>14.2</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>Amery</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>50.4</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>-21.4</t>
-  </si>
-  <si>
-    <t>14.1</t>
-  </si>
-  <si>
-    <t>35.5</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Conger + Tracy/Tremenchus + Shackleton + West + Publications</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>69.4</t>
-  </si>
-  <si>
-    <t>25.4</t>
-  </si>
-  <si>
-    <t>-47.1</t>
-  </si>
-  <si>
-    <t>60.8</t>
-  </si>
-  <si>
-    <t>107.6</t>
-  </si>
-  <si>
-    <t>9.6</t>
-  </si>
-  <si>
-    <t>11.9</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>23.8</t>
-  </si>
-  <si>
-    <t>17.3</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Holmes + Moscow University + Totten + Vincennes</t>
-  </si>
-  <si>
-    <t>162</t>
-  </si>
-  <si>
-    <t>89.1</t>
-  </si>
-  <si>
-    <t>-15.3</t>
-  </si>
-  <si>
-    <t>87.1</t>
-  </si>
-  <si>
-    <t>102.3</t>
-  </si>
-  <si>
-    <t>2.7</t>
-  </si>
-  <si>
-    <t>6.6</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Cook + Ninnis + Mertz + Dibble</t>
-  </si>
-  <si>
-    <t>96.1</t>
-  </si>
-  <si>
-    <t>72.4</t>
-  </si>
-  <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>8.8</t>
-  </si>
-  <si>
-    <t>31.6</t>
-  </si>
-  <si>
-    <t>22.8</t>
-  </si>
-  <si>
-    <t>8.9</t>
-  </si>
-  <si>
-    <t>Aviator + Mariner + Lillie + Rennick</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>-2</t>
-  </si>
-  <si>
-    <t>12.3</t>
-  </si>
-  <si>
-    <t>1.9</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>Drygalski + Nansen</t>
-  </si>
-  <si>
-    <t>10.9</t>
-  </si>
-  <si>
-    <t>-0.4</t>
-  </si>
-  <si>
-    <t>8.7</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>Ross East</t>
-  </si>
-  <si>
-    <t>56.1</t>
-  </si>
-  <si>
-    <t>45.8</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>-7.8</t>
-  </si>
-  <si>
-    <t>41.3</t>
-  </si>
-  <si>
-    <t>49.1</t>
-  </si>
-  <si>
-    <t>Ross West</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>100.4</t>
-  </si>
-  <si>
-    <t>33.5</t>
-  </si>
-  <si>
-    <t>7.6</t>
-  </si>
-  <si>
-    <t>-1.4</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Getz + Land + Nickerson + Sulzberger + Swinburne + Withrow</t>
-  </si>
-  <si>
-    <t>140.3</t>
-  </si>
-  <si>
-    <t>73.7</t>
-  </si>
-  <si>
-    <t>48.8</t>
-  </si>
-  <si>
-    <t>-59.6</t>
-  </si>
-  <si>
-    <t>115.6</t>
-  </si>
-  <si>
-    <t>175.2</t>
-  </si>
-  <si>
-    <t>4.4</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
-    <t>15.6</t>
-  </si>
-  <si>
-    <t>19.9</t>
-  </si>
-  <si>
-    <t>Thwaites + Crosson + Dotson</t>
-  </si>
-  <si>
-    <t>169.3</t>
-  </si>
-  <si>
-    <t>71.7</t>
-  </si>
-  <si>
-    <t>-69.5</t>
-  </si>
-  <si>
-    <t>111.7</t>
-  </si>
-  <si>
-    <t>181.2</t>
-  </si>
-  <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>2.6</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Pine Island</t>
-  </si>
-  <si>
-    <t>126.4</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>4.6</t>
-  </si>
-  <si>
-    <t>-33.2</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>101.2</t>
-  </si>
-  <si>
-    <t>Ferrigno + Venable + Abbot + Cosgrove</t>
-  </si>
-  <si>
-    <t>64.8</t>
-  </si>
-  <si>
-    <t>16.8</t>
-  </si>
-  <si>
-    <t>30.2</t>
-  </si>
-  <si>
-    <t>-6.4</t>
-  </si>
-  <si>
-    <t>78.3</t>
-  </si>
-  <si>
-    <t>84.8</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Wilkins + Bach + George VI + Stange</t>
-  </si>
-  <si>
-    <t>102.4</t>
-  </si>
-  <si>
-    <t>28.8</t>
-  </si>
-  <si>
-    <t>-26.8</t>
-  </si>
-  <si>
-    <t>119.4</t>
-  </si>
-  <si>
-    <t>146.2</t>
-  </si>
-  <si>
-    <t>5.3</t>
-  </si>
-  <si>
-    <t>37.3</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>Wordie</t>
-  </si>
-  <si>
-    <t>13.8</t>
-  </si>
-  <si>
-    <t>-0.1</t>
-  </si>
-  <si>
-    <t>6.5</t>
   </si>
   <si>
     <t>Larsen B + Larsen C + Larsen D + Larsen E + Larsen F</t>
@@ -1469,7 +1457,7 @@
         <v>87</v>
       </c>
       <c r="B8" t="n">
-        <v>1268.83</v>
+        <v>60654</v>
       </c>
       <c r="C8" t="s">
         <v>88</v>
@@ -1487,131 +1475,131 @@
         <v>92</v>
       </c>
       <c r="H8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
         <v>94</v>
       </c>
-      <c r="K8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L8" t="s">
-        <v>91</v>
-      </c>
       <c r="M8" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="N8" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Q8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="R8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="S8" t="e">
-        <v>#NUM!</v>
+        <v>61251.9011285469</v>
+      </c>
+      <c r="P8" t="n">
+        <v>9.55613751829932</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>4.53388137581007</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-0.0263204659354028</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-0.201527118668958</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="n">
+        <v>47688.286</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="B9" t="n">
-        <v>60654</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>98</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>99</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>100</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>101</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>102</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>103</v>
       </c>
-      <c r="I9" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" t="s">
-        <v>60</v>
-      </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="L9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M9" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="N9" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="O9" t="n">
-        <v>61251.9011285469</v>
+        <v>51950.1461442786</v>
       </c>
       <c r="P9" t="n">
-        <v>9.55613751829932</v>
+        <v>15.9230173291997</v>
       </c>
       <c r="Q9" t="n">
-        <v>4.53388137581007</v>
+        <v>10.1324132495254</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.0263204659354028</v>
+        <v>0.0543078687606177</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.201527118668958</v>
+        <v>0.887160695813649</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B10" t="n">
-        <v>47688.286</v>
+        <v>14686.08</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I10" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="K10" t="s">
         <v>114</v>
@@ -1626,19 +1614,19 @@
         <v>117</v>
       </c>
       <c r="O10" t="n">
-        <v>51950.1461442786</v>
+        <v>16872.3759794911</v>
       </c>
       <c r="P10" t="n">
-        <v>15.9230173291997</v>
+        <v>7.49812638441794</v>
       </c>
       <c r="Q10" t="n">
-        <v>10.1324132495254</v>
+        <v>4.68341315050905</v>
       </c>
       <c r="R10" t="n">
-        <v>0.0543078687606177</v>
+        <v>-0.107123286836215</v>
       </c>
       <c r="S10" t="n">
-        <v>0.887160695813649</v>
+        <v>0.133987696763303</v>
       </c>
     </row>
     <row r="11">
@@ -1646,7 +1634,7 @@
         <v>118</v>
       </c>
       <c r="B11" t="n">
-        <v>14686.08</v>
+        <v>12364.85</v>
       </c>
       <c r="C11" t="s">
         <v>119</v>
@@ -1655,639 +1643,639 @@
         <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="K11" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="L11" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="M11" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="N11" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="O11" t="n">
-        <v>16872.3759794911</v>
+        <v>16959.864022457</v>
       </c>
       <c r="P11" t="n">
-        <v>7.49812638441794</v>
+        <v>3.98852361724034</v>
       </c>
       <c r="Q11" t="n">
-        <v>4.68341315050905</v>
+        <v>2.48402355483147</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.107123286836215</v>
+        <v>0.182356090193689</v>
       </c>
       <c r="S11" t="n">
-        <v>0.133987696763303</v>
+        <v>0.546791199701368</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="n">
+        <v>7533.221</v>
+      </c>
+      <c r="C12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" t="s">
         <v>128</v>
       </c>
-      <c r="B12" t="n">
-        <v>12364.85</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>129</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>130</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
         <v>131</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>132</v>
       </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>133</v>
       </c>
-      <c r="H12" t="s">
+      <c r="K12" t="s">
         <v>134</v>
       </c>
-      <c r="I12" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>135</v>
       </c>
-      <c r="K12" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" t="s">
-        <v>84</v>
-      </c>
       <c r="M12" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="N12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O12" t="n">
-        <v>16959.864022457</v>
+        <v>11090.2601270554</v>
       </c>
       <c r="P12" t="n">
-        <v>3.98852361724034</v>
+        <v>1.96565658298567</v>
       </c>
       <c r="Q12" t="n">
-        <v>2.48402355483147</v>
+        <v>1.18327317844996</v>
       </c>
       <c r="R12" t="n">
-        <v>0.182356090193689</v>
+        <v>-0.00150553140795958</v>
       </c>
       <c r="S12" t="n">
-        <v>0.546791199701368</v>
+        <v>0.359043955285426</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B13" t="n">
-        <v>7533.221</v>
+        <v>4323.036</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F13" t="s">
         <v>139</v>
       </c>
       <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
         <v>140</v>
-      </c>
-      <c r="H13" t="s">
-        <v>92</v>
       </c>
       <c r="I13" t="s">
         <v>141</v>
       </c>
       <c r="J13" t="s">
+        <v>141</v>
+      </c>
+      <c r="K13" t="s">
         <v>142</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>143</v>
       </c>
-      <c r="L13" t="s">
-        <v>93</v>
-      </c>
       <c r="M13" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
       <c r="N13" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="O13" t="n">
-        <v>11090.2601270554</v>
+        <v>9672.52537871924</v>
       </c>
       <c r="P13" t="n">
-        <v>1.96565658298567</v>
+        <v>0.276161621538561</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.18327317844996</v>
+        <v>0.340336358082679</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.00150553140795958</v>
+        <v>-0.0471034952284167</v>
       </c>
       <c r="S13" t="n">
-        <v>0.359043955285426</v>
+        <v>0.0447075365362778</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" t="n">
+        <v>194703.9</v>
+      </c>
+      <c r="C14" t="s">
         <v>145</v>
       </c>
-      <c r="B14" t="n">
-        <v>4323.036</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>146</v>
       </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I14" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="J14" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="K14" t="s">
-        <v>149</v>
+        <v>39</v>
       </c>
       <c r="L14" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="M14" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="N14" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="O14" t="n">
-        <v>9672.52537871924</v>
+        <v>261695.84067063</v>
       </c>
       <c r="P14" t="n">
-        <v>0.276161621538561</v>
+        <v>27.973218291374</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.340336358082679</v>
+        <v>31.1542165655646</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0471034952284167</v>
+        <v>-1.00569858386389</v>
       </c>
       <c r="S14" t="n">
-        <v>0.0447075365362778</v>
+        <v>1.79010527727523</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B15" t="n">
-        <v>194703.9</v>
+        <v>306104.618</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G15" t="s">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
         <v>156</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="J15" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="K15" t="s">
         <v>39</v>
       </c>
       <c r="L15" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="M15" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="N15" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="O15" t="n">
-        <v>261695.84067063</v>
+        <v>243421.058624036</v>
       </c>
       <c r="P15" t="n">
-        <v>27.973218291374</v>
+        <v>29.5866885539514</v>
       </c>
       <c r="Q15" t="n">
-        <v>31.1542165655646</v>
+        <v>34.6650130219151</v>
       </c>
       <c r="R15" t="n">
-        <v>-1.00569858386389</v>
+        <v>-0.504770241502507</v>
       </c>
       <c r="S15" t="n">
-        <v>1.79010527727523</v>
+        <v>1.29258191109924</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B16" t="n">
-        <v>306104.618</v>
+        <v>55018.1992</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E16" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F16" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I16" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
+        <v>167</v>
       </c>
       <c r="K16" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="L16" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="M16" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="N16" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="O16" t="n">
-        <v>243421.058624036</v>
+        <v>61251.7422482527</v>
       </c>
       <c r="P16" t="n">
-        <v>29.5866885539514</v>
+        <v>33.5775485292438</v>
       </c>
       <c r="Q16" t="n">
-        <v>34.6650130219151</v>
+        <v>33.2821219259889</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.504770241502507</v>
+        <v>-0.0965518119573875</v>
       </c>
       <c r="S16" t="n">
-        <v>1.29258191109924</v>
+        <v>1.67133399234763</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B17" t="n">
-        <v>55018.1992</v>
+        <v>14530.72</v>
       </c>
       <c r="C17" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E17" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G17" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H17" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="J17" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="K17" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="L17" t="s">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="M17" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="N17" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="O17" t="n">
-        <v>61251.7422482527</v>
+        <v>11270.4765791499</v>
       </c>
       <c r="P17" t="n">
-        <v>33.5775485292438</v>
+        <v>11.9719429209121</v>
       </c>
       <c r="Q17" t="n">
-        <v>33.2821219259889</v>
+        <v>9.49846840877907</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.0965518119573875</v>
+        <v>-0.380865094885242</v>
       </c>
       <c r="S17" t="n">
-        <v>1.67133399234763</v>
+        <v>0.983621683137063</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B18" t="n">
-        <v>14530.72</v>
+        <v>6249.4</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D18" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
       <c r="F18" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="G18" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H18" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="I18" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
       <c r="J18" t="s">
-        <v>183</v>
+        <v>86</v>
       </c>
       <c r="K18" t="s">
-        <v>184</v>
+        <v>85</v>
       </c>
       <c r="L18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M18" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="N18" t="s">
-        <v>185</v>
+        <v>60</v>
       </c>
       <c r="O18" t="n">
-        <v>11270.4765791499</v>
+        <v>8050.02236036435</v>
       </c>
       <c r="P18" t="n">
-        <v>11.9719429209121</v>
+        <v>3.97531225345787</v>
       </c>
       <c r="Q18" t="n">
-        <v>9.49846840877907</v>
+        <v>1.78194823605811</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.380865094885242</v>
+        <v>0.052494606064043</v>
       </c>
       <c r="S18" t="n">
-        <v>0.983621683137063</v>
+        <v>0.685676364111707</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B19" t="n">
-        <v>6249.4</v>
+        <v>36032.6</v>
       </c>
       <c r="C19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G19" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" t="s">
+        <v>177</v>
+      </c>
+      <c r="K19" t="s">
         <v>39</v>
       </c>
-      <c r="J19" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" t="s">
-        <v>85</v>
-      </c>
       <c r="L19" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="M19" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="N19" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="O19" t="n">
-        <v>8050.02236036435</v>
+        <v>39831.5661025749</v>
       </c>
       <c r="P19" t="n">
-        <v>3.97531225345787</v>
+        <v>24.1747992258391</v>
       </c>
       <c r="Q19" t="n">
-        <v>1.78194823605811</v>
+        <v>18.7169119161308</v>
       </c>
       <c r="R19" t="n">
-        <v>0.052494606064043</v>
+        <v>0.733804758149009</v>
       </c>
       <c r="S19" t="n">
-        <v>0.685676364111707</v>
+        <v>5.15812620656883</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B20" t="n">
-        <v>36032.6</v>
+        <v>48905.56</v>
       </c>
       <c r="C20" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D20" t="s">
-        <v>195</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I20" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="J20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="K20" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="L20" t="s">
-        <v>29</v>
+        <v>202</v>
       </c>
       <c r="M20" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="N20" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="O20" t="n">
-        <v>39831.5661025749</v>
+        <v>42746.063428544</v>
       </c>
       <c r="P20" t="n">
-        <v>24.1747992258391</v>
+        <v>27.9019163495893</v>
       </c>
       <c r="Q20" t="n">
-        <v>18.7169119161308</v>
+        <v>17.4042371008088</v>
       </c>
       <c r="R20" t="n">
-        <v>0.733804758149009</v>
+        <v>0.474925798361377</v>
       </c>
       <c r="S20" t="n">
-        <v>5.15812620656883</v>
+        <v>5.53546602482955</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B21" t="n">
-        <v>48905.56</v>
+        <v>276.85</v>
       </c>
       <c r="C21" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
       <c r="F21" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G21" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H21" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I21" t="s">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="J21" t="s">
-        <v>184</v>
+        <v>41</v>
       </c>
       <c r="K21" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="L21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M21" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="N21" t="s">
-        <v>209</v>
+        <v>83</v>
       </c>
       <c r="O21" t="n">
-        <v>42746.063428544</v>
+        <v>3118.87593048901</v>
       </c>
       <c r="P21" t="n">
-        <v>27.9019163495893</v>
+        <v>0.297222919580271</v>
       </c>
       <c r="Q21" t="n">
-        <v>17.4042371008088</v>
+        <v>0.11511694446113</v>
       </c>
       <c r="R21" t="n">
-        <v>0.474925798361377</v>
+        <v>0.00245806771792466</v>
       </c>
       <c r="S21" t="n">
-        <v>5.53546602482955</v>
+        <v>0.0208484662447106</v>
       </c>
     </row>
     <row r="22">
@@ -2295,16 +2283,16 @@
         <v>210</v>
       </c>
       <c r="B22" t="n">
-        <v>276.85</v>
+        <v>77780.2921</v>
       </c>
       <c r="C22" t="s">
         <v>211</v>
       </c>
       <c r="D22" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>202</v>
       </c>
       <c r="F22" t="s">
         <v>212</v>
@@ -2313,157 +2301,98 @@
         <v>213</v>
       </c>
       <c r="H22" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I22" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>215</v>
       </c>
       <c r="K22" t="s">
-        <v>91</v>
+        <v>216</v>
       </c>
       <c r="L22" t="s">
-        <v>91</v>
+        <v>217</v>
       </c>
       <c r="M22" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="N22" t="s">
-        <v>83</v>
+        <v>218</v>
       </c>
       <c r="O22" t="n">
-        <v>3118.87593048901</v>
+        <v>66486.6953527817</v>
       </c>
       <c r="P22" t="n">
-        <v>0.297222919580271</v>
+        <v>34.3363663584496</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.11511694446113</v>
+        <v>38.5337864131377</v>
       </c>
       <c r="R22" t="n">
-        <v>0.00245806771792466</v>
+        <v>0.719217080965996</v>
       </c>
       <c r="S22" t="n">
-        <v>0.0208484662447106</v>
+        <v>-9.35779627619574</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B23" t="n">
-        <v>77780.2921</v>
+        <v>1547105.745</v>
       </c>
       <c r="C23" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>221</v>
       </c>
       <c r="E23" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="F23" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="G23" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="H23" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="I23" t="s">
-        <v>28</v>
+        <v>226</v>
       </c>
       <c r="J23" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="K23" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="L23" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="M23" t="s">
-        <v>92</v>
+        <v>230</v>
       </c>
       <c r="N23" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="O23" t="n">
-        <v>66486.6953527817</v>
+        <v>1602294.1668154</v>
       </c>
       <c r="P23" t="n">
-        <v>34.3363663584496</v>
+        <v>3204588.3336308</v>
       </c>
       <c r="Q23" t="n">
-        <v>38.5337864131377</v>
+        <v>3204952.58756252</v>
       </c>
       <c r="R23" t="n">
-        <v>0.719217080965996</v>
+        <v>3205248.84528162</v>
       </c>
       <c r="S23" t="n">
-        <v>-9.35779627619574</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>223</v>
-      </c>
-      <c r="B24" t="n">
-        <v>1547105.745</v>
-      </c>
-      <c r="C24" t="s">
-        <v>224</v>
-      </c>
-      <c r="D24" t="s">
-        <v>225</v>
-      </c>
-      <c r="E24" t="s">
-        <v>226</v>
-      </c>
-      <c r="F24" t="s">
-        <v>227</v>
-      </c>
-      <c r="G24" t="s">
-        <v>228</v>
-      </c>
-      <c r="H24" t="s">
-        <v>229</v>
-      </c>
-      <c r="I24" t="s">
-        <v>230</v>
-      </c>
-      <c r="J24" t="s">
-        <v>231</v>
-      </c>
-      <c r="K24" t="s">
-        <v>232</v>
-      </c>
-      <c r="L24" t="s">
-        <v>233</v>
-      </c>
-      <c r="M24" t="s">
-        <v>234</v>
-      </c>
-      <c r="N24" t="s">
-        <v>235</v>
-      </c>
-      <c r="O24" t="n">
-        <v>1602294.1668154</v>
-      </c>
-      <c r="P24" t="n">
-        <v>3204588.3336308</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>3204952.58756252</v>
-      </c>
-      <c r="R24" t="n">
-        <v>3205248.84528162</v>
-      </c>
-      <c r="S24" t="n">
         <v>3205255.5879172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Columns sum corrected. Added snow precipitation columns and plots
</commit_message>
<xml_diff>
--- a/output/definitive.xlsx
+++ b/output/definitive.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -71,10 +71,22 @@
     <t>dSMB.A1B.2071.2100.Gt.year</t>
   </si>
   <si>
-    <t>dH.dt.1981.2010.Gt.year</t>
-  </si>
-  <si>
-    <t>dH.dt.A1B.2000.2010.Gt.year</t>
+    <t>SMB.A1B.2001.2030.Gt.year</t>
+  </si>
+  <si>
+    <t>SMB.A1B.2071.2100.Gt.year</t>
+  </si>
+  <si>
+    <t>dH.dt.proj.2001.2030.Gt.year</t>
+  </si>
+  <si>
+    <t>dH.dt.proj.2071.2100.Gt.year</t>
+  </si>
+  <si>
+    <t>Snow.prec.2001.2030.mm.year</t>
+  </si>
+  <si>
+    <t>Snow.prec.2071.2100.mm.year</t>
   </si>
   <si>
     <t>Ronne + Larsen G</t>
@@ -536,10 +548,22 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" t="n">
         <v>339298.57</v>
@@ -596,15 +620,27 @@
         <v>17.338035258348</v>
       </c>
       <c r="T2" t="n">
-        <v>-35.9069782707199</v>
+        <v>63.6212579037088</v>
       </c>
       <c r="U2" t="n">
-        <v>-35.9069782707199</v>
+        <v>76.738035258348</v>
+      </c>
+      <c r="V2" t="n">
+        <v>184.521257903709</v>
+      </c>
+      <c r="W2" t="n">
+        <v>197.638035258348</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-543.831522495685</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-582.490033065415</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" t="n">
         <v>104253.3</v>
@@ -661,15 +697,27 @@
         <v>2.96817759982679</v>
       </c>
       <c r="T3" t="n">
-        <v>-13.3812434332813</v>
+        <v>13.9951919417901</v>
       </c>
       <c r="U3" t="n">
-        <v>-13.3812434332813</v>
+        <v>16.0681775998268</v>
+      </c>
+      <c r="V3" t="n">
+        <v>70.7951919417901</v>
+      </c>
+      <c r="W3" t="n">
+        <v>72.8681775998268</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-679.069074473327</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>-698.953199561326</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
         <v>82499.59</v>
@@ -726,15 +774,27 @@
         <v>1.98311330600375</v>
       </c>
       <c r="T4" t="n">
-        <v>10.7856621901187</v>
+        <v>24.0244524734754</v>
       </c>
       <c r="U4" t="n">
-        <v>10.7856621901187</v>
+        <v>26.5831133060038</v>
+      </c>
+      <c r="V4" t="n">
+        <v>37.1244524734754</v>
+      </c>
+      <c r="W4" t="n">
+        <v>39.6831133060038</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-449.995599656621</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>-481.009824485234</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
         <v>12812.9</v>
@@ -791,15 +851,27 @@
         <v>0.466436060724014</v>
       </c>
       <c r="T5" t="n">
-        <v>3.19495864859462</v>
+        <v>8.37283269330014</v>
       </c>
       <c r="U5" t="n">
-        <v>3.19495864859462</v>
+        <v>8.76643606072401</v>
+      </c>
+      <c r="V5" t="n">
+        <v>13.8728326933001</v>
+      </c>
+      <c r="W5" t="n">
+        <v>14.266436060724</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-1082.72387151232</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-1113.44317529396</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" t="n">
         <v>113268.0357</v>
@@ -856,15 +928,27 @@
         <v>5.17558102116303</v>
       </c>
       <c r="T6" t="n">
-        <v>-8.89234018508736</v>
+        <v>33.2852990878104</v>
       </c>
       <c r="U6" t="n">
-        <v>-8.89234018508736</v>
+        <v>36.575581021163</v>
+      </c>
+      <c r="V6" t="n">
+        <v>119.98529908781</v>
+      </c>
+      <c r="W6" t="n">
+        <v>123.275581021163</v>
+      </c>
+      <c r="X6" t="n">
+        <v>-1059.30413948028</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>-1088.35277542615</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>6852.907</v>
@@ -921,15 +1005,27 @@
         <v>0.472354170205627</v>
       </c>
       <c r="T7" t="n">
-        <v>1.65123431292528</v>
+        <v>4.99397571540916</v>
       </c>
       <c r="U7" t="n">
-        <v>1.65123431292528</v>
+        <v>5.27235417020563</v>
+      </c>
+      <c r="V7" t="n">
+        <v>25.1939757154092</v>
+      </c>
+      <c r="W7" t="n">
+        <v>25.4723541702056</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-3676.39247335608</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>-3717.01442471139</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B8" t="n">
         <v>60654</v>
@@ -986,15 +1082,27 @@
         <v>-0.201527118668958</v>
       </c>
       <c r="T8" t="n">
-        <v>-20.3438624817007</v>
+        <v>8.4736795340646</v>
       </c>
       <c r="U8" t="n">
-        <v>-20.3438624817007</v>
+        <v>8.29847288133104</v>
+      </c>
+      <c r="V8" t="n">
+        <v>49.5736795340646</v>
+      </c>
+      <c r="W8" t="n">
+        <v>49.398472881331</v>
+      </c>
+      <c r="X8" t="n">
+        <v>-817.319212814729</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>-814.430587946896</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
         <v>47688.286</v>
@@ -1051,15 +1159,27 @@
         <v>0.0622336872446787</v>
       </c>
       <c r="T9" t="n">
-        <v>-66.9044044568939</v>
+        <v>25.5136379510608</v>
       </c>
       <c r="U9" t="n">
-        <v>-66.9044044568939</v>
+        <v>25.4622336872447</v>
+      </c>
+      <c r="V9" t="n">
+        <v>168.713637951061</v>
+      </c>
+      <c r="W9" t="n">
+        <v>168.662233687245</v>
+      </c>
+      <c r="X9" t="n">
+        <v>-3537.84235296401</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>-3536.76443072927</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>14686.08</v>
@@ -1116,15 +1236,27 @@
         <v>0.273209923115604</v>
       </c>
       <c r="T10" t="n">
-        <v>-24.4963491047253</v>
+        <v>14.1167246460745</v>
       </c>
       <c r="U10" t="n">
-        <v>-24.4963491047253</v>
+        <v>14.3732099231156</v>
+      </c>
+      <c r="V10" t="n">
+        <v>189.316724646074</v>
+      </c>
+      <c r="W10" t="n">
+        <v>189.573209923116</v>
+      </c>
+      <c r="X10" t="n">
+        <v>-12890.8956403666</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>-12908.3601562238</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11" t="n">
         <v>12364.85</v>
@@ -1181,15 +1313,27 @@
         <v>0.112810074051328</v>
       </c>
       <c r="T11" t="n">
-        <v>7.21299897756038</v>
+        <v>8.00980824200625</v>
       </c>
       <c r="U11" t="n">
-        <v>7.21299897756038</v>
+        <v>8.21281007405133</v>
+      </c>
+      <c r="V11" t="n">
+        <v>54.5098082420062</v>
+      </c>
+      <c r="W11" t="n">
+        <v>54.7128100740513</v>
+      </c>
+      <c r="X11" t="n">
+        <v>-4408.4488078712</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>-4424.86646211247</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" t="n">
         <v>7533.221</v>
@@ -1246,15 +1390,27 @@
         <v>0.333129714327755</v>
       </c>
       <c r="T12" t="n">
-        <v>-1.87001258629171</v>
+        <v>2.31109950611006</v>
       </c>
       <c r="U12" t="n">
-        <v>-1.87001258629171</v>
+        <v>2.53312971432776</v>
+      </c>
+      <c r="V12" t="n">
+        <v>26.4110995061101</v>
+      </c>
+      <c r="W12" t="n">
+        <v>26.6331297143278</v>
+      </c>
+      <c r="X12" t="n">
+        <v>-3505.95044352344</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>-3535.42391950638</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B13" t="n">
         <v>4323.036</v>
@@ -1311,15 +1467,27 @@
         <v>0.206042003053048</v>
       </c>
       <c r="T13" t="n">
-        <v>0.128017374225987</v>
+        <v>0.59913603139006</v>
       </c>
       <c r="U13" t="n">
-        <v>0.128017374225987</v>
+        <v>0.806042003053048</v>
+      </c>
+      <c r="V13" t="n">
+        <v>16.9991360313901</v>
+      </c>
+      <c r="W13" t="n">
+        <v>17.206042003053</v>
+      </c>
+      <c r="X13" t="n">
+        <v>-3932.22171441322</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>-3980.08297942766</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B14" t="n">
         <v>194703.9</v>
@@ -1376,15 +1544,27 @@
         <v>2.01356910352025</v>
       </c>
       <c r="T14" t="n">
-        <v>-26.3620409490271</v>
+        <v>28.8785200436443</v>
       </c>
       <c r="U14" t="n">
-        <v>-26.3620409490271</v>
+        <v>33.0135691035203</v>
+      </c>
+      <c r="V14" t="n">
+        <v>88.2785200436443</v>
+      </c>
+      <c r="W14" t="n">
+        <v>92.4135691035203</v>
+      </c>
+      <c r="X14" t="n">
+        <v>-453.398827879895</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>-474.636456195897</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B15" t="n">
         <v>306104.618</v>
@@ -1441,15 +1621,27 @@
         <v>1.29258191109924</v>
       </c>
       <c r="T15" t="n">
-        <v>3.58668855395137</v>
+        <v>32.9952297584975</v>
       </c>
       <c r="U15" t="n">
-        <v>3.58668855395137</v>
+        <v>34.7925819110992</v>
+      </c>
+      <c r="V15" t="n">
+        <v>4.19522975849748</v>
+      </c>
+      <c r="W15" t="n">
+        <v>5.99258191109923</v>
+      </c>
+      <c r="X15" t="n">
+        <v>-13.7052155106575</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>-19.576907889378</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B16" t="n">
         <v>55018.1992</v>
@@ -1506,15 +1698,27 @@
         <v>0.263808513482053</v>
       </c>
       <c r="T16" t="n">
-        <v>-102.746974145939</v>
+        <v>48.8478199407002</v>
       </c>
       <c r="U16" t="n">
-        <v>-102.746974145939</v>
+        <v>49.0638085134821</v>
+      </c>
+      <c r="V16" t="n">
+        <v>290.6478199407</v>
+      </c>
+      <c r="W16" t="n">
+        <v>290.863808513482</v>
+      </c>
+      <c r="X16" t="n">
+        <v>-5282.75778136883</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>-5286.68354731396</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B17" t="n">
         <v>14530.72</v>
@@ -1571,15 +1775,27 @@
         <v>0.441411871388286</v>
       </c>
       <c r="T17" t="n">
-        <v>-74.7319170191078</v>
+        <v>14.1744999406479</v>
       </c>
       <c r="U17" t="n">
-        <v>-74.7319170191078</v>
+        <v>14.6414118713883</v>
+      </c>
+      <c r="V17" t="n">
+        <v>292.974499940648</v>
+      </c>
+      <c r="W17" t="n">
+        <v>293.441411871388</v>
+      </c>
+      <c r="X17" t="n">
+        <v>-20162.4214038016</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>-20194.5541495114</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B18" t="n">
         <v>6249.4</v>
@@ -1636,15 +1852,27 @@
         <v>0.423037904976268</v>
       </c>
       <c r="T18" t="n">
-        <v>-32.6510837666717</v>
+        <v>4.43619680759275</v>
       </c>
       <c r="U18" t="n">
-        <v>-32.6510837666717</v>
+        <v>5.02303790497627</v>
+      </c>
+      <c r="V18" t="n">
+        <v>169.036196807593</v>
+      </c>
+      <c r="W18" t="n">
+        <v>169.623037904976</v>
+      </c>
+      <c r="X18" t="n">
+        <v>-27048.3881344758</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>-27142.2917248018</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B19" t="n">
         <v>36032.6</v>
@@ -1701,15 +1929,27 @@
         <v>3.95345187657879</v>
       </c>
       <c r="T19" t="n">
-        <v>-13.8792658008855</v>
+        <v>30.5026717992868</v>
       </c>
       <c r="U19" t="n">
-        <v>-13.8792658008855</v>
+        <v>34.1534518765788</v>
+      </c>
+      <c r="V19" t="n">
+        <v>163.302671799287</v>
+      </c>
+      <c r="W19" t="n">
+        <v>166.953451876579</v>
+      </c>
+      <c r="X19" t="n">
+        <v>-4532.08127637991</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>-4633.4000842731</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B20" t="n">
         <v>48905.56</v>
@@ -1766,15 +2006,27 @@
         <v>7.00091169338112</v>
       </c>
       <c r="T20" t="n">
-        <v>-22.7885433183499</v>
+        <v>29.7959628954875</v>
       </c>
       <c r="U20" t="n">
-        <v>-22.7885433183499</v>
+        <v>35.8009116933811</v>
+      </c>
+      <c r="V20" t="n">
+        <v>266.595962895487</v>
+      </c>
+      <c r="W20" t="n">
+        <v>272.600911693381</v>
+      </c>
+      <c r="X20" t="n">
+        <v>-5451.24036807855</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>-5574.02699597717</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B21" t="n">
         <v>276.85</v>
@@ -1831,15 +2083,27 @@
         <v>0.0313357779560046</v>
       </c>
       <c r="T21" t="n">
-        <v>-0.14204974768955</v>
+        <v>0.202688512456996</v>
       </c>
       <c r="U21" t="n">
-        <v>-0.14204974768955</v>
+        <v>0.231335777956005</v>
+      </c>
+      <c r="V21" t="n">
+        <v>12.902688512457</v>
+      </c>
+      <c r="W21" t="n">
+        <v>12.931335777956</v>
+      </c>
+      <c r="X21" t="n">
+        <v>-46605.3404820553</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>-46708.8162469063</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B22" t="n">
         <v>77780.2921</v>
@@ -1896,54 +2160,66 @@
         <v>-9.35779627619574</v>
       </c>
       <c r="T22" t="n">
-        <v>14.9363663584496</v>
+        <v>38.019217080966</v>
       </c>
       <c r="U22" t="n">
-        <v>14.9363663584496</v>
+        <v>27.9422037238043</v>
+      </c>
+      <c r="V22" t="n">
+        <v>93.819217080966</v>
+      </c>
+      <c r="W22" t="n">
+        <v>83.7422037238043</v>
+      </c>
+      <c r="X22" t="n">
+        <v>-1206.20808366656</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>-1076.65067156265</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B23" t="n">
-        <v>1547105.745</v>
+        <v>1545836.915</v>
       </c>
       <c r="C23" t="n">
-        <v>5088</v>
+        <v>1681.6</v>
       </c>
       <c r="D23" t="n">
-        <v>3268.1</v>
+        <v>1088</v>
       </c>
       <c r="E23" t="n">
-        <v>1291.1</v>
+        <v>429.1</v>
       </c>
       <c r="F23" t="n">
-        <v>-861.4</v>
+        <v>-287.4</v>
       </c>
       <c r="G23" t="n">
-        <v>3111.3</v>
+        <v>1023.1</v>
       </c>
       <c r="H23" t="n">
-        <v>3974.2</v>
+        <v>1310</v>
       </c>
       <c r="I23" t="n">
-        <v>436.2</v>
+        <v>135.9</v>
       </c>
       <c r="J23" t="n">
-        <v>407.6</v>
+        <v>128.1</v>
       </c>
       <c r="K23" t="n">
-        <v>242.5</v>
+        <v>79.4</v>
       </c>
       <c r="L23" t="n">
-        <v>566.9</v>
+        <v>333.9</v>
       </c>
       <c r="M23" t="n">
-        <v>646.5</v>
+        <v>203.1</v>
       </c>
       <c r="N23" t="n">
-        <v>944.4</v>
+        <v>423</v>
       </c>
       <c r="O23" t="n">
         <v>1445329.43903024</v>
@@ -1961,10 +2237,22 @@
         <v>35.2519080755809</v>
       </c>
       <c r="T23" t="n">
-        <v>-1841.50113885054</v>
+        <v>435.16990250548</v>
       </c>
       <c r="U23" t="n">
-        <v>-1841.50113885054</v>
+        <v>464.351908075581</v>
+      </c>
+      <c r="V23" t="n">
+        <v>2338.76990250548</v>
+      </c>
+      <c r="W23" t="n">
+        <v>2367.95190807558</v>
+      </c>
+      <c r="X23" t="n">
+        <v>-1512.94737485647</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>-1531.82517838603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plots with region labels
</commit_message>
<xml_diff>
--- a/output/definitive.xlsx
+++ b/output/definitive.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>dH.dt.proj.2071.2100.Gt.year</t>
+  </si>
+  <si>
+    <t>Current.snow.prec.offset.mm.year</t>
   </si>
   <si>
     <t>Snow.prec.2001.2030.mm.year</t>
@@ -560,10 +563,13 @@
       <c r="Y1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="n">
         <v>339298.57</v>
@@ -632,15 +638,18 @@
         <v>197.638035258348</v>
       </c>
       <c r="X2" t="n">
+        <v>139.699969852511</v>
+      </c>
+      <c r="Y2" t="n">
         <v>-543.831522495685</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Z2" t="n">
         <v>-582.490033065415</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" t="n">
         <v>104253.3</v>
@@ -709,15 +718,18 @@
         <v>72.8681775998268</v>
       </c>
       <c r="X3" t="n">
+        <v>130.451506091414</v>
+      </c>
+      <c r="Y3" t="n">
         <v>-679.069074473327</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="Z3" t="n">
         <v>-698.953199561326</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
         <v>82499.59</v>
@@ -786,15 +798,18 @@
         <v>39.6831133060038</v>
       </c>
       <c r="X4" t="n">
+        <v>-187.879721584071</v>
+      </c>
+      <c r="Y4" t="n">
         <v>-449.995599656621</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="Z4" t="n">
         <v>-481.009824485234</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" t="n">
         <v>12812.9</v>
@@ -863,15 +878,18 @@
         <v>14.266436060724</v>
       </c>
       <c r="X5" t="n">
+        <v>-624.370751352153</v>
+      </c>
+      <c r="Y5" t="n">
         <v>-1082.72387151232</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="Z5" t="n">
         <v>-1113.44317529396</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" t="n">
         <v>113268.0357</v>
@@ -940,15 +958,18 @@
         <v>123.275581021163</v>
       </c>
       <c r="X6" t="n">
+        <v>-13.2429241023732</v>
+      </c>
+      <c r="Y6" t="n">
         <v>-1059.30413948028</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="Z6" t="n">
         <v>-1088.35277542615</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" t="n">
         <v>6852.907</v>
@@ -1017,15 +1038,18 @@
         <v>25.4723541702056</v>
       </c>
       <c r="X7" t="n">
+        <v>-583.693898078582</v>
+      </c>
+      <c r="Y7" t="n">
         <v>-3676.39247335608</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="Z7" t="n">
         <v>-3717.01442471139</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="n">
         <v>60654</v>
@@ -1094,15 +1118,18 @@
         <v>49.398472881331</v>
       </c>
       <c r="X8" t="n">
+        <v>352.820918653345</v>
+      </c>
+      <c r="Y8" t="n">
         <v>-817.319212814729</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="Z8" t="n">
         <v>-814.430587946896</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="n">
         <v>47688.286</v>
@@ -1171,15 +1198,18 @@
         <v>168.662233687245</v>
       </c>
       <c r="X9" t="n">
+        <v>987.663930718751</v>
+      </c>
+      <c r="Y9" t="n">
         <v>-3537.84235296401</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="Z9" t="n">
         <v>-3536.76443072927</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" t="n">
         <v>14686.08</v>
@@ -1248,15 +1278,18 @@
         <v>189.573209923116</v>
       </c>
       <c r="X10" t="n">
+        <v>1041.80285004576</v>
+      </c>
+      <c r="Y10" t="n">
         <v>-12890.8956403666</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="Z10" t="n">
         <v>-12908.3601562238</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="n">
         <v>12364.85</v>
@@ -1325,15 +1358,18 @@
         <v>54.7128100740513</v>
       </c>
       <c r="X11" t="n">
+        <v>-711.694844660469</v>
+      </c>
+      <c r="Y11" t="n">
         <v>-4408.4488078712</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="Z11" t="n">
         <v>-4424.86646211247</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" t="n">
         <v>7533.221</v>
@@ -1402,15 +1438,18 @@
         <v>26.6331297143278</v>
       </c>
       <c r="X12" t="n">
+        <v>265.490684529234</v>
+      </c>
+      <c r="Y12" t="n">
         <v>-3505.95044352344</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="Z12" t="n">
         <v>-3535.42391950638</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" t="n">
         <v>4323.036</v>
@@ -1479,15 +1518,18 @@
         <v>17.206042003053</v>
       </c>
       <c r="X13" t="n">
+        <v>92.5275662751825</v>
+      </c>
+      <c r="Y13" t="n">
         <v>-3932.22171441322</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="Z13" t="n">
         <v>-3980.08297942766</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="n">
         <v>194703.9</v>
@@ -1556,15 +1598,18 @@
         <v>92.4135691035203</v>
       </c>
       <c r="X14" t="n">
+        <v>40.0608308308154</v>
+      </c>
+      <c r="Y14" t="n">
         <v>-453.398827879895</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="Z14" t="n">
         <v>-474.636456195897</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" t="n">
         <v>306104.618</v>
@@ -1633,15 +1678,18 @@
         <v>5.99258191109923</v>
       </c>
       <c r="X15" t="n">
+        <v>-24.8281128512736</v>
+      </c>
+      <c r="Y15" t="n">
         <v>-13.7052155106575</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="Z15" t="n">
         <v>-19.576907889378</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" t="n">
         <v>55018.1992</v>
@@ -1710,15 +1758,18 @@
         <v>290.863808513482</v>
       </c>
       <c r="X16" t="n">
+        <v>1083.27791288378</v>
+      </c>
+      <c r="Y16" t="n">
         <v>-5282.75778136883</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="Z16" t="n">
         <v>-5286.68354731396</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" t="n">
         <v>14530.72</v>
@@ -1787,15 +1838,18 @@
         <v>293.441411871388</v>
       </c>
       <c r="X17" t="n">
+        <v>4782.97014876069</v>
+      </c>
+      <c r="Y17" t="n">
         <v>-20162.4214038016</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="Z17" t="n">
         <v>-20194.5541495114</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" t="n">
         <v>6249.4</v>
@@ -1864,15 +1918,18 @@
         <v>169.623037904976</v>
       </c>
       <c r="X18" t="n">
+        <v>5312.51000096009</v>
+      </c>
+      <c r="Y18" t="n">
         <v>-27048.3881344758</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="Z18" t="n">
         <v>-27142.2917248018</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" t="n">
         <v>36032.6</v>
@@ -1941,15 +1998,18 @@
         <v>166.953451876579</v>
       </c>
       <c r="X19" t="n">
+        <v>177.616935774826</v>
+      </c>
+      <c r="Y19" t="n">
         <v>-4532.08127637991</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="Z19" t="n">
         <v>-4633.4000842731</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20" t="n">
         <v>48905.56</v>
@@ -2018,15 +2078,18 @@
         <v>272.600911693381</v>
       </c>
       <c r="X20" t="n">
+        <v>547.994951903219</v>
+      </c>
+      <c r="Y20" t="n">
         <v>-5451.24036807855</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="Z20" t="n">
         <v>-5574.02699597717</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" t="n">
         <v>276.85</v>
@@ -2095,15 +2158,18 @@
         <v>12.931335777956</v>
       </c>
       <c r="X21" t="n">
+        <v>361.206429474445</v>
+      </c>
+      <c r="Y21" t="n">
         <v>-46605.3404820553</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="Z21" t="n">
         <v>-46708.8162469063</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B22" t="n">
         <v>77780.2921</v>
@@ -2172,15 +2238,18 @@
         <v>83.7422037238043</v>
       </c>
       <c r="X22" t="n">
+        <v>-228.849744831442</v>
+      </c>
+      <c r="Y22" t="n">
         <v>-1206.20808366656</v>
       </c>
-      <c r="Y22" t="n">
+      <c r="Z22" t="n">
         <v>-1076.65067156265</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23" t="n">
         <v>1545836.915</v>
@@ -2249,9 +2318,12 @@
         <v>2367.95190807558</v>
       </c>
       <c r="X23" t="n">
+        <v>185.918706696172</v>
+      </c>
+      <c r="Y23" t="n">
         <v>-1512.94737485647</v>
       </c>
-      <c r="Y23" t="n">
+      <c r="Z23" t="n">
         <v>-1531.82517838603</v>
       </c>
     </row>

</xml_diff>